<commit_message>
ödev 1 ve ödev 2 düzenleme commit
</commit_message>
<xml_diff>
--- a/data/invalidCredentials.xlsx
+++ b/data/invalidCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMET\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA64C7D-9F62-4259-BFBB-774135A65CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC1C3D-EC28-4DC5-B47E-EE9E0175D380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25155" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>password</t>
   </si>
@@ -36,13 +36,19 @@
     <t>problem user</t>
   </si>
   <si>
-    <t>aaaaaa</t>
-  </si>
-  <si>
     <t>deneme</t>
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>naber</t>
+  </si>
+  <si>
+    <t>nasilsin</t>
+  </si>
+  <si>
+    <t>nerde</t>
   </si>
 </sst>
 </file>
@@ -400,7 +406,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,11 +424,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -430,15 +436,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>